<commit_message>
-Add filter for Application Date From and Application Date To -Add order by -Remove Project desc.,Res of enf. action ,city jur. appr req. and City uti. app. req. -Add AssessorParcelNumber, ApplicationDate.
</commit_message>
<xml_diff>
--- a/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/BuildingModuleTemplate.xlsx
+++ b/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/BuildingModuleTemplate.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Type</t>
   </si>
@@ -39,31 +36,31 @@
     <t>Application Name</t>
   </si>
   <si>
-    <t>Project Description</t>
-  </si>
-  <si>
     <t>Office Project Description</t>
   </si>
   <si>
     <t>Contractor Name</t>
   </si>
   <si>
-    <t>Res. Of Enf. Action</t>
-  </si>
-  <si>
-    <t>City Jur. App. Req</t>
-  </si>
-  <si>
-    <t>City Utility App. Req.</t>
-  </si>
-  <si>
     <t>App #</t>
+  </si>
+  <si>
+    <t>Application Date</t>
+  </si>
+  <si>
+    <t>Issue Date</t>
+  </si>
+  <si>
+    <t>Assessor Parcel Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,6 +124,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -410,67 +413,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="23.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="15.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="15.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>